<commit_message>
Object cat added to InOut, InOutAddition now fetches teams that are in Object
</commit_message>
<xml_diff>
--- a/pkg/excels/templates/Шаблон для импорта КЛ 04 КВ.xlsx
+++ b/pkg/excels/templates/Шаблон для импорта КЛ 04 КВ.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mamad\OneDrive\Desktop\ТГЭМ\backend-v2\pkg\excels\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BA6D26-5DBB-4E1C-BB54-E4ABA318B927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Импорт" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Имя</t>
   </si>
@@ -44,11 +45,11 @@
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <sz val="12"/>
         <scheme val="minor"/>
       </rPr>
       <t>*</t>
@@ -60,11 +61,11 @@
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <sz val="12"/>
         <scheme val="minor"/>
       </rPr>
       <t>*</t>
@@ -76,11 +77,11 @@
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <sz val="12"/>
         <scheme val="minor"/>
       </rPr>
       <t>*</t>
@@ -92,41 +93,22 @@
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <sz val="12"/>
         <scheme val="minor"/>
       </rPr>
       <t>*</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>Супервайзер</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <sz val="12"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <t>Исфандиёр</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,7 +117,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -143,7 +125,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -151,7 +133,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -181,14 +163,14 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -201,7 +183,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -463,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,7 +459,7 @@
     <col min="4" max="5" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -485,12 +467,9 @@
         <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -527,35 +506,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097094F9-7E6F-44E4-B859-0524084CD09F}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Update 1.3.4: Changes to reference books
</commit_message>
<xml_diff>
--- a/pkg/excels/templates/Шаблон для импорта КЛ 04 КВ.xlsx
+++ b/pkg/excels/templates/Шаблон для импорта КЛ 04 КВ.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mamad\OneDrive\Desktop\ТГЭМ\backend-v2\pkg\excels\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BA6D26-5DBB-4E1C-BB54-E4ABA318B927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="Импорт" sheetId="1" r:id="rId1"/>
-    <sheet name="Супервайзеры" sheetId="2" r:id="rId2"/>
+    <sheet name="КЛ 04 КВ" sheetId="1" r:id="rId1"/>
+    <sheet name="ТП" sheetId="4" r:id="rId2"/>
+    <sheet name="Бригады" sheetId="3" r:id="rId3"/>
+    <sheet name="Супервайзеры" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,30 +27,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
-  <si>
-    <t>Имя</t>
-  </si>
-  <si>
-    <t>Сиаваш</t>
-  </si>
-  <si>
-    <t>Шахзод</t>
-  </si>
-  <si>
-    <t>Мурод</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <r>
       <t>Наимнование</t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <sz val="12"/>
         <scheme val="minor"/>
       </rPr>
       <t>*</t>
@@ -61,11 +50,11 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <sz val="12"/>
         <scheme val="minor"/>
       </rPr>
       <t>*</t>
@@ -77,38 +66,74 @@
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <sz val="12"/>
         <scheme val="minor"/>
       </rPr>
       <t>*</t>
     </r>
   </si>
   <si>
-    <r>
-      <t>Длина</t>
+    <t>Супервайзер</t>
+  </si>
+  <si>
+    <t>Бригада</t>
+  </si>
+  <si>
+    <t>Питается от ТП</t>
+  </si>
+  <si>
+    <r>
+      <t>Длина линии</t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <sz val="12"/>
         <scheme val="minor"/>
       </rPr>
       <t>*</t>
     </r>
   </si>
+  <si>
+    <t>Номер Бригады</t>
+  </si>
+  <si>
+    <t>Наименование ТП</t>
+  </si>
+  <si>
+    <t>Имя Супервайзера</t>
+  </si>
+  <si>
+    <t>Мурод</t>
+  </si>
+  <si>
+    <t>Бригада-04</t>
+  </si>
+  <si>
+    <t>Бригада-03</t>
+  </si>
+  <si>
+    <t>Бригада-02</t>
+  </si>
+  <si>
+    <t>Бригада-01</t>
+  </si>
+  <si>
+    <t>Вилка</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,7 +142,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -125,7 +150,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -133,7 +158,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -163,14 +188,14 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -183,7 +208,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -445,32 +470,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="195" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -478,25 +514,31 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B159" xr:uid="{97E180B8-70D3-40D7-9813-50FDDD79F612}">
       <formula1>"  В ожидании, Идет работа, Работа завершена,   Сдано заказчику,"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D47 E2:E126" xr:uid="{369879D8-D174-4EAD-B927-0696E229D932}">
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D47" xr:uid="{369879D8-D174-4EAD-B927-0696E229D932}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BEF7AA8-B587-4114-8370-3FF93C5AD676}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3181346C-CC42-4750-8688-BB2516E0A62F}">
           <x14:formula1>
-            <xm:f>Супервайзеры!$A$2:$A$220</xm:f>
+            <xm:f>Супервайзеры!$A$2:$A$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>E127:E131</xm:sqref>
+          <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F8D1B3DC-4DE7-4F45-ACEC-014DB6ED8F00}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F938E719-33A7-4FAB-ABBC-7940B49535BA}">
           <x14:formula1>
-            <xm:f>Супервайзеры!$A$2:$A$58</xm:f>
+            <xm:f>Бригады!$A$2:$A$1048576</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C157</xm:sqref>
+          <xm:sqref>F2:F1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8CBE3260-A7B9-4A79-B012-0FBF9F5CAF27}">
+          <x14:formula1>
+            <xm:f>ТП!$A$2:$A$1048576</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -505,38 +547,93 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097094F9-7E6F-44E4-B859-0524084CD09F}">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE49D96-2421-478C-A81D-644762B95458}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" s="1" customFormat="true">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{916CEC8F-5959-4F21-A0A6-FBF4F72235BF}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col bestFit="true" customWidth="true" max="1" min="1" width="15.44140625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097094F9-7E6F-44E4-B859-0524084CD09F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>